<commit_message>
Added scroll opacity directive
Added scroll opacity directive
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Homepage</t>
   </si>
   <si>
-    <t>Update Homepage with new info, video etc.</t>
-  </si>
-  <si>
     <t>Add Google chart to Homepage</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Daterange picker - values, dates to angular controller</t>
   </si>
   <si>
-    <t>Fade in Divs as scroll down.</t>
-  </si>
-  <si>
     <t>Validation logic and add modelstate errors etc.</t>
   </si>
   <si>
@@ -252,6 +246,15 @@
   </si>
   <si>
     <t>Change page size, number results, e.g. 15, 20 etc.</t>
+  </si>
+  <si>
+    <t>Fade in - scroll directive opacity - added</t>
+  </si>
+  <si>
+    <t>Finishs update - complete text, fa icons etc</t>
+  </si>
+  <si>
+    <t>Added more unit tests for text search</t>
   </si>
 </sst>
 </file>
@@ -399,9 +402,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -699,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J50"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,40 +713,40 @@
     <col min="3" max="3" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="76.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>40</v>
+      <c r="I2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>42773</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
@@ -755,10 +757,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>42773</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
@@ -769,10 +771,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>42773</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G6" t="s">
@@ -783,10 +785,10 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>42774</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
@@ -797,10 +799,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>42774</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
@@ -811,18 +813,18 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>42774</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>42774</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
@@ -833,192 +835,202 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>42774</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G11" t="s">
         <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>42775</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>42775</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G13" t="s">
         <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>42775</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
       </c>
       <c r="H14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>42776</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>42776</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>42776</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>42776</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>37</v>
       </c>
-      <c r="H16" t="s">
+    </row>
+    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>42777</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>42777</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>42777</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>42777</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" t="s">
-        <v>39</v>
-      </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>42778</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>42778</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>42778</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>42779</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>42779</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>42780</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
         <v>46</v>
       </c>
-      <c r="H20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>42778</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <v>42779</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>42779</v>
-      </c>
-      <c r="C23" s="3" t="s">
+    </row>
+    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>42780</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>42780</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
-        <v>42780</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
       <c r="H25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>42781</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>42782</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="H27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1033,17 +1045,17 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.25">
@@ -1053,51 +1065,46 @@
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>66</v>
+      </c>
       <c r="H48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G50" t="s">
-        <v>68</v>
-      </c>
-      <c r="H50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new pages - checkout & confirmation
Added new pages - checkout & confirmation, recommended rentals updated,
new date picker shows start and end dates
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Backlog</t>
-  </si>
-  <si>
-    <t>Add Wishlist to Identity Table for AspNetUser</t>
   </si>
   <si>
     <t>Feature</t>
@@ -155,9 +152,6 @@
     <t>Recommended</t>
   </si>
   <si>
-    <t>Show Recommended &amp; similar cars on Bottom Detail Page</t>
-  </si>
-  <si>
     <t>Reviews</t>
   </si>
   <si>
@@ -188,12 +182,6 @@
     <t>Special Offer</t>
   </si>
   <si>
-    <t>Add appstrap shop-checkout Page</t>
-  </si>
-  <si>
-    <t>Add appstrap shop-confirmation Page</t>
-  </si>
-  <si>
     <t>Email With Confirmation - and PDF Invoice</t>
   </si>
   <si>
@@ -255,6 +243,27 @@
   </si>
   <si>
     <t>Added more unit tests for text search</t>
+  </si>
+  <si>
+    <t>Added and updated search Pagination</t>
+  </si>
+  <si>
+    <t>Add Wishlist Table - AspNetUser Id and Car ID</t>
+  </si>
+  <si>
+    <t>Added Recommended Rentals to Details page - static</t>
+  </si>
+  <si>
+    <t>Recommended &amp; similar cars (dynamic from api controller) Details Page</t>
+  </si>
+  <si>
+    <t>Add appstrap shop-checkout &amp; confirmation pages static</t>
+  </si>
+  <si>
+    <t>Added new date picker - displays start and end dates</t>
+  </si>
+  <si>
+    <t>Make checkout &amp; confirmation pages dynamic</t>
   </si>
 </sst>
 </file>
@@ -701,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J48"/>
+  <dimension ref="B1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,16 +735,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -750,10 +759,10 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -764,10 +773,10 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -778,10 +787,10 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -792,10 +801,10 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -806,10 +815,10 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -828,10 +837,10 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
         <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -842,10 +851,10 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -864,10 +873,10 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -878,10 +887,10 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
         <v>34</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -900,10 +909,10 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -922,10 +931,10 @@
         <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -944,10 +953,10 @@
         <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -955,13 +964,13 @@
         <v>42778</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -969,13 +978,7 @@
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -983,7 +986,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -991,13 +1000,13 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1005,13 +1014,7 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1019,7 +1022,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1027,84 +1033,105 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>42782</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>42782</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>42782</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>42782</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="H31" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
-        <v>41</v>
-      </c>
-      <c r="H40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G48" t="s">
-        <v>66</v>
-      </c>
-      <c r="H48" t="s">
-        <v>67</v>
+      <c r="H47" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added wishlistController and updated pagination links
Added wishlistController and updated pagination links
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>Make checkout &amp; confirmation pages dynamic</t>
+  </si>
+  <si>
+    <t>Pagination page links - SO question - (created Plunker)</t>
+  </si>
+  <si>
+    <t>Go direct to certain page - eg pg 17</t>
+  </si>
+  <si>
+    <t>Added wishlistController and sharedProperties to get &amp; set carId</t>
   </si>
 </sst>
 </file>
@@ -710,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,27 +1089,39 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>42783</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>42783</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="H33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
         <v>39</v>
       </c>
@@ -1108,17 +1129,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>51</v>
       </c>
@@ -1126,12 +1147,20 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>62</v>
       </c>
       <c r="H47" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkout & Confirmation pages working
Checkout & Confirmation pages working
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -276,6 +276,18 @@
   </si>
   <si>
     <t>Added Log In and Register pages - static</t>
+  </si>
+  <si>
+    <t>Admin Area</t>
+  </si>
+  <si>
+    <t>Update cars etc.</t>
+  </si>
+  <si>
+    <t>Register working - user added to AspNetUser table</t>
+  </si>
+  <si>
+    <t>Checkout populated from View Model</t>
   </si>
 </sst>
 </file>
@@ -707,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I49"/>
+  <dimension ref="B1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1113,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>42785</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>42787</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H36" t="s">
         <v>37</v>
       </c>
@@ -1154,6 +1180,14 @@
       </c>
       <c r="H49" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pageSelectionSize drop down working
pageSelectionSize drop down working
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -137,9 +137,6 @@
     <t>User can log in from modal</t>
   </si>
   <si>
-    <t>Finish Categories Sidebar and css class issue?</t>
-  </si>
-  <si>
     <t>AutoComplete on text boxes???</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Fade in - scroll directive opacity - added</t>
   </si>
   <si>
-    <t>Finishs update - complete text, fa icons etc</t>
-  </si>
-  <si>
     <t>Added more unit tests for text search</t>
   </si>
   <si>
@@ -288,6 +282,27 @@
   </si>
   <si>
     <t>Checkout populated from View Model</t>
+  </si>
+  <si>
+    <t>Checkout &amp; Confirmation Pages Working</t>
+  </si>
+  <si>
+    <t>Search DDL's - only use values when $dirty flagged</t>
+  </si>
+  <si>
+    <t>Populate DDLS from API calls</t>
+  </si>
+  <si>
+    <t>Filter DDLs by other selections?</t>
+  </si>
+  <si>
+    <t>Finish update - complete text, fa icons etc</t>
+  </si>
+  <si>
+    <t>Finish Categories Sidebar</t>
+  </si>
+  <si>
+    <t>Footer links</t>
   </si>
 </sst>
 </file>
@@ -719,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I51"/>
+  <dimension ref="B1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,12 +746,12 @@
     <col min="3" max="3" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="76.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -750,14 +765,14 @@
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>42773</v>
       </c>
@@ -768,10 +783,13 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>42773</v>
       </c>
@@ -784,8 +802,11 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>42773</v>
       </c>
@@ -798,8 +819,11 @@
       <c r="H6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>42774</v>
       </c>
@@ -813,7 +837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>42774</v>
       </c>
@@ -827,7 +851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>42774</v>
       </c>
@@ -835,7 +859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>42774</v>
       </c>
@@ -849,7 +873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>42774</v>
       </c>
@@ -857,7 +881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>42775</v>
       </c>
@@ -865,13 +889,13 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>42775</v>
       </c>
@@ -879,13 +903,13 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>42775</v>
       </c>
@@ -893,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>42776</v>
       </c>
@@ -901,13 +925,13 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>42776</v>
       </c>
@@ -923,10 +947,10 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -945,10 +969,10 @@
         <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -959,10 +983,10 @@
         <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -972,19 +996,19 @@
       <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -992,13 +1016,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1006,7 +1030,13 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="G24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1014,10 +1044,7 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1025,10 +1052,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H26" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,10 +1063,10 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1047,7 +1074,10 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1055,10 +1085,10 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1066,10 +1096,7 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1077,10 +1104,10 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1088,10 +1115,10 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H32" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1099,7 +1126,10 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1107,10 +1137,10 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H34" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1118,7 +1148,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1126,68 +1156,74 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>42787</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>42788</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G38" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G47" t="s">
-        <v>60</v>
-      </c>
-      <c r="H47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G49" t="s">
-        <v>74</v>
-      </c>
-      <c r="H49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H51" t="s">
-        <v>79</v>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>76</v>
+      </c>
+      <c r="H50" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 x Advanced Search DDLs working
3 x Advanced Search DDLs working
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Footer links</t>
+  </si>
+  <si>
+    <t>Refactor - carListController logic - single method</t>
   </si>
 </sst>
 </file>
@@ -737,7 +740,7 @@
   <dimension ref="B1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,6 +853,9 @@
       <c r="H8" t="s">
         <v>27</v>
       </c>
+      <c r="J8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">

</xml_diff>

<commit_message>
Added login service and recieves token
Added login service and recieves token
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Go direct to certain page - eg pg 17</t>
   </si>
   <si>
-    <t>Logging</t>
-  </si>
-  <si>
     <t>Log errors with Nlog?</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
     <t>Search DDL's - only use values when $dirty flagged</t>
   </si>
   <si>
-    <t>Populate DDLS from API calls</t>
-  </si>
-  <si>
     <t>Filter DDLs by other selections?</t>
   </si>
   <si>
@@ -306,6 +300,27 @@
   </si>
   <si>
     <t>Refactor - carListController logic - single method</t>
+  </si>
+  <si>
+    <t>3 x Advanced Search DDLS working</t>
+  </si>
+  <si>
+    <t>Moved calendar and drop downs - Details layout</t>
+  </si>
+  <si>
+    <t>Error Logging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Call to carDropDown controller to get values</t>
+  </si>
+  <si>
+    <t>Remove all junk words from TextSearch method…</t>
+  </si>
+  <si>
+    <t>Added login service and working - can get token</t>
+  </si>
+  <si>
+    <t>Add second footer with no links - updated info</t>
   </si>
 </sst>
 </file>
@@ -789,7 +804,7 @@
         <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -806,7 +821,7 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -822,9 +837,6 @@
       <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -839,6 +851,9 @@
       <c r="H7" t="s">
         <v>24</v>
       </c>
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -853,9 +868,6 @@
       <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="J8" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -864,6 +876,9 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="J9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -878,6 +893,9 @@
       <c r="H10" t="s">
         <v>30</v>
       </c>
+      <c r="J10" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -898,7 +916,13 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -914,6 +938,9 @@
       <c r="H13" t="s">
         <v>33</v>
       </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -1072,7 +1099,7 @@
         <v>61</v>
       </c>
       <c r="H27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1094,7 +1121,7 @@
         <v>65</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1132,7 +1159,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H33" t="s">
         <v>55</v>
@@ -1143,7 +1170,7 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H34" t="s">
         <v>31</v>
@@ -1154,7 +1181,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1162,7 +1189,7 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H36" t="s">
         <v>47</v>
@@ -1173,7 +1200,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1187,12 +1214,34 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>42788</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>42789</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
       <c r="H40" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>42789</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -1218,18 +1267,18 @@
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" t="s">
         <v>72</v>
-      </c>
-      <c r="H48" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" t="s">
         <v>76</v>
-      </c>
-      <c r="H50" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change image API to use google custom search
Change image API to use google custom search
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Add second footer with no links - updated info</t>
+  </si>
+  <si>
+    <t>Add Exception handling - add to db</t>
   </si>
 </sst>
 </file>
@@ -752,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J50"/>
+  <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,6 +1284,11 @@
         <v>76</v>
       </c>
     </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added stored proc and NewSearchController
Added stored proc and NewSearchController
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>Add Exception handling - add to db</t>
+  </si>
+  <si>
+    <t>Add rental orders to the Db</t>
+  </si>
+  <si>
+    <t>Add token to http requests - $http interceptor</t>
+  </si>
+  <si>
+    <t>Show all favourites in top drop down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - Show 5 favourites - paginate?</t>
+  </si>
+  <si>
+    <t>Search remove junk words - DropDownListController</t>
   </si>
 </sst>
 </file>
@@ -458,7 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -471,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -757,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +786,7 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="76.7109375" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="45.42578125" customWidth="1"/>
+    <col min="10" max="10" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -974,8 +992,11 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J16" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>42777</v>
       </c>
@@ -989,15 +1010,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>42777</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J18" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>42778</v>
       </c>
@@ -1011,7 +1035,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>42778</v>
       </c>
@@ -1024,8 +1048,11 @@
       <c r="H20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J20" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>42778</v>
       </c>
@@ -1038,16 +1065,22 @@
       <c r="H21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J21" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>42779</v>
       </c>
@@ -1061,7 +1094,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>42780</v>
       </c>
@@ -1075,7 +1108,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>42780</v>
       </c>
@@ -1083,7 +1116,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>42781</v>
       </c>
@@ -1094,7 +1127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>42782</v>
       </c>
@@ -1105,7 +1138,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>42782</v>
       </c>
@@ -1116,7 +1149,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>42782</v>
       </c>
@@ -1127,7 +1160,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>42782</v>
       </c>
@@ -1135,7 +1168,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>42782</v>
       </c>
@@ -1146,7 +1179,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>42783</v>
       </c>

</xml_diff>

<commit_message>
CarSearchController now uses stored procedure
CarSearchController now uses stored procedure - removed old search utility
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -309,12 +309,6 @@
   </si>
   <si>
     <t>Error Logging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   - Call to carDropDown controller to get values</t>
-  </si>
-  <si>
-    <t>Remove all junk words from TextSearch method…</t>
   </si>
   <si>
     <t>Added login service and working - can get token</t>
@@ -773,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J52"/>
+  <dimension ref="B1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,9 +891,6 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -915,7 +906,7 @@
         <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -942,9 +933,6 @@
       <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -970,6 +958,9 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="J14" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -993,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1018,7 +1009,7 @@
         <v>18</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1034,6 +1025,9 @@
       <c r="H19" t="s">
         <v>69</v>
       </c>
+      <c r="J19" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
@@ -1065,9 +1059,6 @@
       <c r="H21" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
@@ -1076,9 +1067,6 @@
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
@@ -1093,6 +1081,9 @@
       <c r="H23" t="s">
         <v>41</v>
       </c>
+      <c r="J23" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
@@ -1277,7 +1268,7 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -1315,11 +1306,6 @@
       </c>
       <c r="H50" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H52" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemneted favouritedetailscontroller and count
implemneted favouritedetailscontroller - returning count and cars json to view
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Hook up link to show Wishlist and display</t>
   </si>
   <si>
-    <t>WishList</t>
-  </si>
-  <si>
-    <t>Ad to Wishlist - adds record to Db</t>
-  </si>
-  <si>
     <t>Remove from WishList - remove from Db</t>
   </si>
   <si>
@@ -236,9 +230,6 @@
     <t>Added and updated search Pagination</t>
   </si>
   <si>
-    <t>Add Wishlist Table - AspNetUser Id and Car ID</t>
-  </si>
-  <si>
     <t>Added Recommended Rentals to Details page - static</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
   </si>
   <si>
     <t xml:space="preserve">  - Show 5 favourites - paginate?</t>
-  </si>
-  <si>
-    <t>Search remove junk words - DropDownListController</t>
   </si>
 </sst>
 </file>
@@ -767,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J50"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +786,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -816,10 +804,10 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -830,13 +818,13 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -850,7 +838,7 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -860,14 +848,8 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -878,10 +860,10 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -900,13 +882,13 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="J10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -916,6 +898,12 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -924,12 +912,6 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" t="s">
-        <v>82</v>
-      </c>
       <c r="I12" s="5">
         <v>1</v>
       </c>
@@ -945,7 +927,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="I13" s="5">
         <v>1</v>
@@ -959,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -970,10 +952,10 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -984,7 +966,7 @@
         <v>14</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -995,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1008,8 +990,14 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
       <c r="J18" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1020,13 +1008,13 @@
         <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,36 +1024,34 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" t="s">
-        <v>43</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>42778</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
         <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>50</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="G22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1073,16 +1059,10 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="J23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1090,13 +1070,10 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1104,7 +1081,10 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1112,10 +1092,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1123,10 +1103,10 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1134,10 +1114,7 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1145,10 +1122,10 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H29" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1156,7 +1133,10 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="H30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1164,10 +1144,10 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H31" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1175,10 +1155,10 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H32" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1186,10 +1166,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1197,10 +1174,10 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H34" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1208,7 +1185,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1216,10 +1193,10 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H36" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1227,7 +1204,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1235,10 +1212,13 @@
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G38" t="s">
+        <v>35</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1246,7 +1226,7 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1254,13 +1234,10 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" t="s">
         <v>37</v>
-      </c>
-      <c r="H40" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1268,44 +1245,39 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
       <c r="H42" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H44" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="H46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="H48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G50" t="s">
-        <v>75</v>
-      </c>
-      <c r="H50" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating favourites on add and added toastr-angular
Updating favourites on add and added toastr-angular
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -308,16 +308,28 @@
     <t>Add token to http requests - $http interceptor</t>
   </si>
   <si>
-    <t>Show all favourites in top drop down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Show 5 favourites - paginate?</t>
-  </si>
-  <si>
     <t>Favourites</t>
   </si>
   <si>
     <t>Show 3 x Toastr notifications</t>
+  </si>
+  <si>
+    <t>Limit favourites drop down to show first 5</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Send email on registration</t>
+  </si>
+  <si>
+    <t>Send email on mailing list sign up</t>
+  </si>
+  <si>
+    <t>Add missing CarInfo entries</t>
+  </si>
+  <si>
+    <t>Show 10,15,20 etc from DDL selection</t>
   </si>
 </sst>
 </file>
@@ -752,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -815,10 +827,10 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>75</v>
@@ -909,8 +921,8 @@
       <c r="H12" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="5">
-        <v>1</v>
+      <c r="J12" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -920,9 +932,6 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -938,7 +947,7 @@
         <v>33</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -962,9 +971,7 @@
       <c r="H16" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -979,6 +986,9 @@
       <c r="H17" t="s">
         <v>38</v>
       </c>
+      <c r="J17" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
@@ -993,9 +1003,6 @@
       <c r="H18" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
@@ -1004,8 +1011,8 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>89</v>
+      <c r="J19" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1035,7 +1042,9 @@
       <c r="H21" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="7"/>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
@@ -1056,7 +1065,7 @@
         <v>46</v>
       </c>
       <c r="J23" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1069,6 +1078,9 @@
       <c r="H24" t="s">
         <v>77</v>
       </c>
+      <c r="J24" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
@@ -1091,6 +1103,9 @@
       <c r="H26" t="s">
         <v>78</v>
       </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
@@ -1121,6 +1136,9 @@
       <c r="H29" t="s">
         <v>48</v>
       </c>
+      <c r="J29" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
@@ -1159,8 +1177,11 @@
       <c r="C33" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
       <c r="H33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1178,8 +1199,11 @@
       <c r="C35" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="G35" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1198,10 +1222,10 @@
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H37" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1219,8 +1243,11 @@
       <c r="C39" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="G39" t="s">
+        <v>82</v>
+      </c>
       <c r="H39" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1239,34 +1266,26 @@
         <v>83</v>
       </c>
       <c r="G41" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H41" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="H43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
-        <v>82</v>
-      </c>
-      <c r="H45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G47" t="s">
-        <v>69</v>
-      </c>
-      <c r="H47" t="s">
-        <v>70</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Order Entity, Repository & api controller
Added Order Entity, Repository & api controller
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Special Offer</t>
   </si>
   <si>
-    <t>Email With Confirmation - and PDF Invoice</t>
-  </si>
-  <si>
     <t>Return IHttpActionResult from apiControllers  - Ok, Bad Result etc.</t>
   </si>
   <si>
@@ -311,9 +308,6 @@
     <t>Favourites</t>
   </si>
   <si>
-    <t>Show 3 x Toastr notifications</t>
-  </si>
-  <si>
     <t>Limit favourites drop down to show first 5</t>
   </si>
   <si>
@@ -330,6 +324,18 @@
   </si>
   <si>
     <t>Show 10,15,20 etc from DDL selection</t>
+  </si>
+  <si>
+    <t>1) ORDERS</t>
+  </si>
+  <si>
+    <t>2) Recommended - 6 x random cars from  Api Controller</t>
+  </si>
+  <si>
+    <t>Email With Confirmation - and PDF Invoice - confirmation GUID</t>
+  </si>
+  <si>
+    <t>2b) Update _Recommended partial view</t>
   </si>
 </sst>
 </file>
@@ -764,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J44"/>
+  <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -810,13 +816,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -826,14 +832,8 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" t="s">
-        <v>89</v>
-      </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -843,6 +843,12 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -851,14 +857,8 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -868,6 +868,12 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -880,7 +886,10 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -890,15 +899,6 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -907,6 +907,15 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -915,15 +924,6 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -932,6 +932,13 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -940,14 +947,8 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
       <c r="J14" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -957,6 +958,12 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -969,9 +976,11 @@
         <v>35</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="J16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -984,10 +993,7 @@
         <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -997,11 +1003,8 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" t="s">
-        <v>45</v>
+      <c r="J18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1011,8 +1014,11 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J19" t="s">
-        <v>85</v>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1026,7 +1032,10 @@
         <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,14 +1045,8 @@
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" t="s">
-        <v>40</v>
-      </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1051,7 +1054,10 @@
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1059,13 +1065,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="J23" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1073,13 +1079,10 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J24" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1087,10 +1090,10 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1098,13 +1101,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,10 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1120,10 +1123,13 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1131,13 +1137,13 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1145,10 +1151,13 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H30" t="s">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1156,10 +1165,10 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H31" t="s">
-        <v>26</v>
+        <v>61</v>
+      </c>
+      <c r="J31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1167,7 +1176,13 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1175,13 +1190,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1189,7 +1198,13 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="G34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1197,13 +1212,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H35" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1211,7 +1220,13 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="G36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1219,13 +1234,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" t="s">
-        <v>54</v>
-      </c>
-      <c r="H37" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1233,7 +1242,13 @@
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="G38" t="s">
+        <v>81</v>
+      </c>
+      <c r="H38" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1241,13 +1256,7 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G39" t="s">
-        <v>82</v>
-      </c>
-      <c r="H39" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1255,7 +1264,13 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1263,29 +1278,23 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G41" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H42" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" t="s">
         <v>91</v>
-      </c>
-      <c r="H43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G44" t="s">
-        <v>91</v>
-      </c>
-      <c r="H44" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Advanced search Drop downs refined onchange
Advanced search Drop downs refined onchange
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>Add Heart &amp; Heart-o - When users adds it chage fa icon</t>
   </si>
   <si>
     <r>
@@ -140,9 +137,6 @@
     <t>Add Car List as Grid View</t>
   </si>
   <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>Reviews - and Ratings - Stars fa icons</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>link to special offer/ featuredlist on click Call To Action Links</t>
   </si>
   <si>
-    <t>Add Search Bar - 3 x Drop Down Lists - filtered by each selection, make, model, year</t>
-  </si>
-  <si>
     <t>Check Thumbnail pics for cars - and change ones not adequate</t>
   </si>
   <si>
@@ -263,12 +254,6 @@
     <t>Checkout &amp; Confirmation Pages Working</t>
   </si>
   <si>
-    <t>Search DDL's - only use values when $dirty flagged</t>
-  </si>
-  <si>
-    <t>Filter DDLs by other selections?</t>
-  </si>
-  <si>
     <t>Finish update - complete text, fa icons etc</t>
   </si>
   <si>
@@ -278,9 +263,6 @@
     <t>Footer links</t>
   </si>
   <si>
-    <t>Refactor - carListController logic - single method</t>
-  </si>
-  <si>
     <t>3 x Advanced Search DDLS working</t>
   </si>
   <si>
@@ -299,9 +281,6 @@
     <t>Add Exception handling - add to db</t>
   </si>
   <si>
-    <t>Add rental orders to the Db</t>
-  </si>
-  <si>
     <t>Add token to http requests - $http interceptor</t>
   </si>
   <si>
@@ -323,12 +302,6 @@
     <t>Add missing CarInfo entries</t>
   </si>
   <si>
-    <t>Show 10,15,20 etc from DDL selection</t>
-  </si>
-  <si>
-    <t>1) ORDERS</t>
-  </si>
-  <si>
     <t>2) Recommended - 6 x random cars from  Api Controller</t>
   </si>
   <si>
@@ -336,6 +309,24 @@
   </si>
   <si>
     <t>2b) Update _Recommended partial view</t>
+  </si>
+  <si>
+    <t>1) ORDERS - Add rental orders to the Db</t>
+  </si>
+  <si>
+    <t>Filter Advanced Search DDLs by other selections</t>
+  </si>
+  <si>
+    <t>Show recommended on Index when logged in</t>
+  </si>
+  <si>
+    <t>Add,remove - When users adds it changes fa icon &amp; link text</t>
+  </si>
+  <si>
+    <t>Log out - implement</t>
+  </si>
+  <si>
+    <t>Create 'My account page'</t>
   </si>
 </sst>
 </file>
@@ -770,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J43"/>
+  <dimension ref="B1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -816,13 +807,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -832,9 +823,6 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -844,10 +832,13 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>25</v>
+      <c r="J6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -857,9 +848,6 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -869,10 +857,13 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -883,13 +874,10 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
         <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -899,6 +887,7 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -908,13 +897,13 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -933,12 +922,14 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -947,9 +938,6 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -959,10 +947,13 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -973,13 +964,10 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -990,10 +978,13 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="J17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1004,7 +995,7 @@
         <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1015,10 +1006,10 @@
         <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1029,13 +1020,13 @@
         <v>17</v>
       </c>
       <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
         <v>37</v>
       </c>
-      <c r="H20" t="s">
-        <v>39</v>
-      </c>
       <c r="J20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1043,10 +1034,7 @@
         <v>42778</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1054,10 +1042,10 @@
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1065,13 +1053,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1079,10 +1067,13 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1090,10 +1081,13 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1101,10 +1095,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1112,10 +1106,10 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1123,13 +1117,10 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1137,13 +1128,10 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>49</v>
-      </c>
-      <c r="J29" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1151,13 +1139,10 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1165,10 +1150,7 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1176,13 +1158,13 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1190,7 +1172,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1198,13 +1180,13 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1212,7 +1194,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1220,13 +1202,13 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G36" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1234,7 +1216,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1242,13 +1224,13 @@
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="H38" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1256,7 +1238,7 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1264,13 +1246,13 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="H40" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1278,23 +1260,23 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G42" t="s">
-        <v>89</v>
-      </c>
-      <c r="H42" t="s">
-        <v>90</v>
+      <c r="H41" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G43" t="s">
-        <v>89</v>
-      </c>
       <c r="H43" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recommended Jobs implemented now from api controller
Recommended Jobs implemented now from api controller
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Added Recommended Rentals to Details page - static</t>
   </si>
   <si>
-    <t>Recommended &amp; similar cars (dynamic from api controller) Details Page</t>
-  </si>
-  <si>
     <t>Add appstrap shop-checkout &amp; confirmation pages static</t>
   </si>
   <si>
@@ -302,31 +299,31 @@
     <t>Add missing CarInfo entries</t>
   </si>
   <si>
-    <t>2) Recommended - 6 x random cars from  Api Controller</t>
-  </si>
-  <si>
     <t>Email With Confirmation - and PDF Invoice - confirmation GUID</t>
   </si>
   <si>
-    <t>2b) Update _Recommended partial view</t>
-  </si>
-  <si>
     <t>1) ORDERS - Add rental orders to the Db</t>
   </si>
   <si>
-    <t>Filter Advanced Search DDLs by other selections</t>
-  </si>
-  <si>
-    <t>Show recommended on Index when logged in</t>
-  </si>
-  <si>
     <t>Add,remove - When users adds it changes fa icon &amp; link text</t>
   </si>
   <si>
     <t>Log out - implement</t>
   </si>
   <si>
-    <t>Create 'My account page'</t>
+    <t>Drop cookie using ngcookies - $cookieStore</t>
+  </si>
+  <si>
+    <t>CarInfo - add for each individual car in list</t>
+  </si>
+  <si>
+    <t>Create 'My account page' - switch on/off Recommended cars</t>
+  </si>
+  <si>
+    <t>Remove email adress from URLS - cookies</t>
+  </si>
+  <si>
+    <t>Recommended cars more tailored to users favourite cars</t>
   </si>
 </sst>
 </file>
@@ -761,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J44"/>
+  <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,13 +804,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -837,8 +834,8 @@
       <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" t="s">
-        <v>77</v>
+      <c r="J6" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -848,6 +845,9 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="J7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -860,11 +860,9 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -879,6 +877,9 @@
       <c r="H9" t="s">
         <v>27</v>
       </c>
+      <c r="J9" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -887,7 +888,6 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -897,13 +897,13 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>81</v>
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -922,13 +922,13 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -938,6 +938,12 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -950,10 +956,10 @@
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -963,11 +969,8 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
+      <c r="J16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -978,13 +981,10 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -994,8 +994,14 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>37</v>
+      </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1005,12 +1011,6 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
@@ -1019,14 +1019,8 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
       <c r="H20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,6 +1030,12 @@
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="H21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
@@ -1045,7 +1045,10 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>42</v>
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1058,9 +1061,6 @@
       <c r="H23" t="s">
         <v>71</v>
       </c>
-      <c r="J23" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
@@ -1069,11 +1069,8 @@
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H24" t="s">
-        <v>21</v>
-      </c>
       <c r="J24" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1084,7 +1081,7 @@
         <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="J25" t="s">
         <v>88</v>
@@ -1097,8 +1094,8 @@
       <c r="C26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J26" t="s">
-        <v>91</v>
+      <c r="H26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1109,7 +1106,10 @@
         <v>52</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1130,19 +1130,19 @@
       <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H29" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>39</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1158,13 +1158,13 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
         <v>60</v>
-      </c>
-      <c r="G32" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1180,10 +1180,10 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H34" t="s">
         <v>61</v>
@@ -1194,7 +1194,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1202,13 +1202,13 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1227,10 +1227,10 @@
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="H38" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,13 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="G39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1246,13 +1252,7 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G40" t="s">
-        <v>82</v>
-      </c>
-      <c r="H40" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1260,23 +1260,13 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G41" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="H41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H43" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login & Logout set and remove cookie
Login & Logout set and remove cookie for email
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -308,22 +308,16 @@
     <t>Add,remove - When users adds it changes fa icon &amp; link text</t>
   </si>
   <si>
-    <t>Log out - implement</t>
-  </si>
-  <si>
-    <t>Drop cookie using ngcookies - $cookieStore</t>
-  </si>
-  <si>
     <t>CarInfo - add for each individual car in list</t>
   </si>
   <si>
     <t>Create 'My account page' - switch on/off Recommended cars</t>
   </si>
   <si>
-    <t>Remove email adress from URLS - cookies</t>
-  </si>
-  <si>
     <t>Recommended cars more tailored to users favourite cars</t>
+  </si>
+  <si>
+    <t>Encrypt cookie</t>
   </si>
 </sst>
 </file>
@@ -845,9 +839,6 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -862,7 +853,9 @@
       <c r="H8" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="J8" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -877,9 +870,6 @@
       <c r="H9" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -888,6 +878,9 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -902,9 +895,6 @@
       <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="J11" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -913,6 +903,9 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -927,9 +920,6 @@
       <c r="H13" t="s">
         <v>58</v>
       </c>
-      <c r="J13" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -944,6 +934,9 @@
       <c r="H14" t="s">
         <v>85</v>
       </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -959,7 +952,7 @@
         <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -969,9 +962,6 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J16" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -986,6 +976,9 @@
       <c r="H17" t="s">
         <v>34</v>
       </c>
+      <c r="J17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
@@ -1000,9 +993,6 @@
       <c r="H18" t="s">
         <v>37</v>
       </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
@@ -1022,6 +1012,9 @@
       <c r="H20" t="s">
         <v>42</v>
       </c>
+      <c r="J20" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -1034,7 +1027,7 @@
         <v>70</v>
       </c>
       <c r="J21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1047,9 +1040,6 @@
       <c r="H22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
@@ -1061,6 +1051,9 @@
       <c r="H23" t="s">
         <v>71</v>
       </c>
+      <c r="J23" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
@@ -1069,9 +1062,6 @@
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J24" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
@@ -1084,7 +1074,7 @@
         <v>36</v>
       </c>
       <c r="J25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1108,9 +1098,6 @@
       <c r="H27" t="s">
         <v>46</v>
       </c>
-      <c r="J27" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
@@ -1266,7 +1253,7 @@
         <v>28</v>
       </c>
       <c r="H41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkout & price calculation implemented
Checkout & price calculation implemented
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Trending Now</t>
   </si>
   <si>
-    <t>Checkout</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add Bool for Featured Cars, Cars On special </t>
   </si>
   <si>
@@ -318,6 +315,15 @@
   </si>
   <si>
     <t>Encrypt cookie</t>
+  </si>
+  <si>
+    <t>Grid View</t>
+  </si>
+  <si>
+    <t>Add Address to Db - Edit from My Account</t>
+  </si>
+  <si>
+    <t>Add Payment Details to DB - Edit from My Account</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
   <dimension ref="B1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,9 +769,9 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="76.7109375" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="56.28515625" customWidth="1"/>
+    <col min="10" max="10" width="79.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -783,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -798,13 +804,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -829,7 +835,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -851,10 +857,10 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -879,7 +885,7 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -915,10 +921,10 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
         <v>33</v>
-      </c>
-      <c r="H13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -929,13 +935,13 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -945,14 +951,8 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>41</v>
-      </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -962,6 +962,9 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -970,14 +973,11 @@
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -987,11 +987,8 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
       <c r="H18" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1001,6 +998,12 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="H19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
@@ -1009,12 +1012,6 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H20" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -1024,10 +1021,7 @@
         <v>22</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1035,10 +1029,10 @@
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1046,13 +1040,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="J23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1060,7 +1054,13 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1068,13 +1068,7 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1082,10 +1076,16 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="J26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1093,10 +1093,10 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="J27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1104,10 +1104,16 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="G28" t="s">
+        <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1115,7 +1121,7 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1123,13 +1129,16 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>43</v>
+        <v>60</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1137,7 +1146,10 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="J31" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1145,13 +1157,13 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="H32" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1159,7 +1171,7 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1167,13 +1179,13 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1181,7 +1193,13 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="G35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1189,13 +1207,7 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1203,7 +1215,13 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1211,13 +1229,7 @@
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" t="s">
-        <v>81</v>
-      </c>
-      <c r="H38" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1225,13 +1237,13 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H39" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1239,7 +1251,7 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1247,13 +1259,7 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G41" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Orders to Db implemented
Adding Orders to Db implemented
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Cost Of Rental and calculate based on special offers etc - Update Cost to rent per week</t>
-  </si>
-  <si>
     <t>Daterange picker - values, dates to angular controller</t>
   </si>
   <si>
@@ -324,6 +321,12 @@
   </si>
   <si>
     <t>Add Payment Details to DB - Edit from My Account</t>
+  </si>
+  <si>
+    <t>Checkout Discount code</t>
+  </si>
+  <si>
+    <t>Notify user if no end date selected at checkout</t>
   </si>
 </sst>
 </file>
@@ -761,7 +764,7 @@
   <dimension ref="B1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,13 +807,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -835,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -857,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -885,7 +888,7 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -952,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -963,7 +966,7 @@
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -974,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -999,10 +1002,10 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1023,16 +1026,22 @@
       <c r="H21" t="s">
         <v>35</v>
       </c>
+      <c r="J21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1040,13 +1049,10 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
-      </c>
-      <c r="J23" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1054,13 +1060,13 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H24" t="s">
         <v>25</v>
       </c>
       <c r="J24" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1068,7 +1074,10 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="J25" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1076,16 +1085,13 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
         <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
-      </c>
-      <c r="J26" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1093,10 +1099,7 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1104,16 +1107,16 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1121,7 +1124,10 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1129,16 +1135,13 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1146,7 +1149,7 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J31" t="s">
         <v>93</v>
@@ -1157,109 +1160,112 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" t="s">
         <v>63</v>
       </c>
-      <c r="H32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G34" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" t="s">
         <v>80</v>
       </c>
-      <c r="H34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G37" t="s">
         <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MyAccount - Orders & Favourites
Added MyAccount - Orders & Favourites
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Daterange picker - values, dates to angular controller</t>
-  </si>
-  <si>
     <t>Validation logic and add modelstate errors etc.</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>Added new date picker - displays start and end dates</t>
   </si>
   <si>
-    <t>Make checkout &amp; confirmation pages dynamic</t>
-  </si>
-  <si>
     <t>Pagination page links - SO question - (created Plunker)</t>
   </si>
   <si>
@@ -251,9 +245,6 @@
     <t>Finish Categories Sidebar</t>
   </si>
   <si>
-    <t>Footer links</t>
-  </si>
-  <si>
     <t>3 x Advanced Search DDLS working</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Email With Confirmation - and PDF Invoice - confirmation GUID</t>
   </si>
   <si>
-    <t>1) ORDERS - Add rental orders to the Db</t>
-  </si>
-  <si>
     <t>Add,remove - When users adds it changes fa icon &amp; link text</t>
   </si>
   <si>
@@ -311,9 +299,6 @@
     <t>Recommended cars more tailored to users favourite cars</t>
   </si>
   <si>
-    <t>Encrypt cookie</t>
-  </si>
-  <si>
     <t>Grid View</t>
   </si>
   <si>
@@ -323,10 +308,28 @@
     <t>Add Payment Details to DB - Edit from My Account</t>
   </si>
   <si>
-    <t>Checkout Discount code</t>
-  </si>
-  <si>
     <t>Notify user if no end date selected at checkout</t>
+  </si>
+  <si>
+    <t>Bug: Add recommended cars to cookie</t>
+  </si>
+  <si>
+    <t>Checkout Discount code - show discounted amount in checkout and Confirmation screens</t>
+  </si>
+  <si>
+    <t>Refactor: Run everything off of "Search"</t>
+  </si>
+  <si>
+    <t>Cost per day per car - different amounts e.g. Category A, B , C</t>
+  </si>
+  <si>
+    <t>See github commits</t>
+  </si>
+  <si>
+    <t>Encrypt cookies</t>
+  </si>
+  <si>
+    <t>Check Footer links</t>
   </si>
 </sst>
 </file>
@@ -761,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J41"/>
+  <dimension ref="B1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -838,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -860,10 +863,10 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -888,7 +891,7 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -955,7 +958,7 @@
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -966,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -977,10 +980,10 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -991,7 +994,7 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1001,11 +1004,8 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
       <c r="J19" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1015,6 +1015,9 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -1024,10 +1027,10 @@
         <v>22</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1035,13 +1038,10 @@
         <v>42779</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="s">
         <v>43</v>
-      </c>
-      <c r="H22" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1049,10 +1049,13 @@
         <v>42779</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>44</v>
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1060,13 +1063,7 @@
         <v>42780</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1074,10 +1071,13 @@
         <v>42780</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" t="s">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1085,13 +1085,10 @@
         <v>42781</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="J26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1099,7 +1096,16 @@
         <v>42782</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="G27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1107,16 +1113,7 @@
         <v>42782</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" t="s">
-        <v>58</v>
-      </c>
-      <c r="J28" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1124,10 +1121,16 @@
         <v>42782</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
       </c>
       <c r="J29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1135,13 +1138,7 @@
         <v>42782</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" t="s">
-        <v>72</v>
-      </c>
-      <c r="H30" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1149,10 +1146,16 @@
         <v>42782</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" t="s">
+        <v>61</v>
       </c>
       <c r="J31" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1160,13 +1163,7 @@
         <v>42783</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G32" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1174,10 +1171,16 @@
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" t="s">
+        <v>77</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1185,13 +1188,16 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="J34" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1199,13 +1205,7 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,16 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>84</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1221,13 +1230,7 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1235,7 +1238,13 @@
         <v>42788</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1243,13 +1252,7 @@
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H39" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1257,7 +1260,7 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1265,7 +1268,12 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insurance popover, End Data and Favoutite link logic on Details page
Insurance popover, End Data and Favoutite link logic on Details page
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Go direct to certain page - eg pg 17</t>
   </si>
   <si>
-    <t>Log errors with Nlog?</t>
-  </si>
-  <si>
     <t>Added wishlistController and can get carId's from link click - Details &amp; List</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>Add Payment Details to DB - Edit from My Account</t>
   </si>
   <si>
-    <t>Notify user if no end date selected at checkout</t>
-  </si>
-  <si>
     <t>Bug: Add recommended cars to cookie</t>
   </si>
   <si>
@@ -330,6 +324,21 @@
   </si>
   <si>
     <t>Check Footer links</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Change from email address to ASPnet_Users table ID</t>
+  </si>
+  <si>
+    <t>Mega Menu Links</t>
+  </si>
+  <si>
+    <t>Implement 'RemoveFavourite' from Details &amp; Index</t>
+  </si>
+  <si>
+    <t>Log errors with NLog?</t>
   </si>
 </sst>
 </file>
@@ -767,7 +776,7 @@
   <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,13 +819,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -826,6 +835,12 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -834,14 +849,8 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -851,6 +860,12 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -859,14 +874,8 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
       <c r="J8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -880,7 +889,7 @@
         <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -890,8 +899,14 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
       <c r="J10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -901,12 +916,6 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -915,6 +924,12 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
       <c r="J12" t="s">
         <v>32</v>
       </c>
@@ -926,12 +941,6 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -944,7 +953,7 @@
         <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J14" t="s">
         <v>37</v>
@@ -957,8 +966,14 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -968,9 +983,6 @@
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H16" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -980,10 +992,10 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -994,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1004,8 +1016,11 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
       <c r="J19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1015,9 +1030,6 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H20" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -1027,10 +1039,10 @@
         <v>22</v>
       </c>
       <c r="H21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1041,7 +1053,7 @@
         <v>42</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1052,10 +1064,10 @@
         <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="J23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1065,6 +1077,9 @@
       <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
@@ -1073,12 +1088,6 @@
       <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
@@ -1087,8 +1096,14 @@
       <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" t="s">
+        <v>40</v>
+      </c>
       <c r="J26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1098,14 +1113,8 @@
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
       <c r="J27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1115,6 +1124,12 @@
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
@@ -1123,14 +1138,8 @@
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G29" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" t="s">
-        <v>57</v>
-      </c>
       <c r="J29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1140,6 +1149,12 @@
       <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
@@ -1148,14 +1163,8 @@
       <c r="C31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" t="s">
-        <v>61</v>
-      </c>
       <c r="J31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1165,22 +1174,22 @@
       <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="G32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>42783</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" t="s">
-        <v>76</v>
-      </c>
-      <c r="H33" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1188,16 +1197,16 @@
         <v>42784</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34" t="s">
         <v>76</v>
       </c>
-      <c r="H34" t="s">
-        <v>78</v>
-      </c>
       <c r="J34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1205,7 +1214,13 @@
         <v>42785</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="G35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1213,16 +1228,10 @@
         <v>42787</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="J36" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1230,7 +1239,13 @@
         <v>42787</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1240,19 +1255,19 @@
       <c r="C38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="39" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>42788</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1260,7 +1275,7 @@
         <v>42789</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1268,12 +1283,18 @@
         <v>42789</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="G41" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MyAccount Index and show hide header icons
Added MyAccount Index and show hide header icons
</commit_message>
<xml_diff>
--- a/Documentation/ActionDiary.xlsx
+++ b/Documentation/ActionDiary.xlsx
@@ -266,9 +266,6 @@
     <t>Favourites</t>
   </si>
   <si>
-    <t>Limit favourites drop down to show first 5</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>Log errors with NLog?</t>
+  </si>
+  <si>
+    <t>Limit favourites drop down to show first 5 - pagination</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
         <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
         <v>70</v>
@@ -839,7 +839,7 @@
         <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>36</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>65</v>
       </c>
       <c r="J17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
         <v>43</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>40</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>49</v>
       </c>
       <c r="J27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>52</v>
       </c>
       <c r="J29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>68</v>
       </c>
       <c r="H30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>54</v>
       </c>
       <c r="J31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1200,13 +1200,13 @@
         <v>58</v>
       </c>
       <c r="G34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" t="s">
         <v>75</v>
       </c>
-      <c r="H34" t="s">
-        <v>76</v>
-      </c>
       <c r="J34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1217,10 +1217,10 @@
         <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>62</v>
       </c>
       <c r="J36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>66</v>
       </c>
       <c r="G39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" t="s">
         <v>30</v>
@@ -1286,15 +1286,15 @@
         <v>69</v>
       </c>
       <c r="G41" t="s">
+        <v>93</v>
+      </c>
+      <c r="H41" t="s">
         <v>94</v>
-      </c>
-      <c r="H41" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>